<commit_message>
1.5.6 fix parasite matching for host.parasite file
</commit_message>
<xml_diff>
--- a/data/smallerb.xlsx
+++ b/data/smallerb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianyandell/Documents/Research/ewing/ewing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47407C3-DD27-9D4F-9EFD-5B56F5D90472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125680CF-9BDD-9746-9E86-53973D9412FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65960" yWindow="2200" windowWidth="14420" windowHeight="17440" xr2:uid="{2A60D24C-DC64-C449-84DD-C019D084A238}"/>
+    <workbookView xWindow="69280" yWindow="460" windowWidth="14420" windowHeight="17440" activeTab="3" xr2:uid="{2A60D24C-DC64-C449-84DD-C019D084A238}"/>
   </bookViews>
   <sheets>
     <sheet name="organism.features" sheetId="1" r:id="rId1"/>
@@ -642,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8956A585-82A1-4C49-A77C-0D68492FFCAA}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1202,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EBC24A-F31B-4D46-863C-6C8374FE545E}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>

</xml_diff>